<commit_message>
Import Trassenköö': Anpassung an iGeo Version 1.2.2 incl. Unterstützung aller (neuen) Felder und Format A0
</commit_message>
<xml_diff>
--- a/GeoTools_cfg.xlsx
+++ b/GeoTools_cfg.xlsx
@@ -11,7 +11,7 @@
     <sheet name="SpaltenKonfig" sheetId="17" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$B$14:$G$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SpaltenKonfig!$B$14:$G$98</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="0">Einstellungen!$A$4:$C$4</definedName>
     <definedName name="Daten.InfoTraeger" localSheetId="1">SpaltenKonfig!$B$15:$G$15</definedName>
     <definedName name="Spalte.Beschreibung" localSheetId="1">SpaltenKonfig!$C$15</definedName>
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="297">
   <si>
     <t>GK.X</t>
   </si>
@@ -1280,6 +1280,36 @@
   </si>
   <si>
     <t>Abwicklungsmass bei Gleisprofil</t>
+  </si>
+  <si>
+    <t>TK.QGT</t>
+  </si>
+  <si>
+    <t>TK.HGT</t>
+  </si>
+  <si>
+    <t>TK.QGS</t>
+  </si>
+  <si>
+    <t>TK.HGS</t>
+  </si>
+  <si>
+    <t>TK.KmStatus</t>
+  </si>
+  <si>
+    <t>Quer im Tunnelsystem</t>
+  </si>
+  <si>
+    <t>Hoch im Tunnelsystem</t>
+  </si>
+  <si>
+    <t>Quer im Strassensystem</t>
+  </si>
+  <si>
+    <t>Hoch im Strassensystem</t>
+  </si>
+  <si>
+    <t>Status des Kilometers (TK.Km)</t>
   </si>
 </sst>
 </file>
@@ -1896,8 +1926,8 @@
         <a:xfrm>
           <a:off x="8678333" y="0"/>
           <a:ext cx="0" cy="0"/>
-          <a:chOff x="731" y="282"/>
-          <a:chExt cx="410" cy="168"/>
+          <a:chOff x="731" y="0"/>
+          <a:chExt cx="8677602" cy="450"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp macro="" textlink="">
@@ -1950,8 +1980,8 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="747" y="282"/>
-                <a:ext cx="374" cy="152"/>
+                <a:off x="8678333" y="0"/>
+                <a:ext cx="0" cy="0"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
@@ -3243,7 +3273,7 @@
   <sheetPr codeName="tabSpaltenGlobal11">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <selection sqref="A1:G1"/>
@@ -4293,21 +4323,17 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="26">
+      <c r="A62" s="1">
         <v>48</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>11</v>
+        <v>291</v>
       </c>
       <c r="C62" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E62" s="28" t="s">
-        <v>6</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
       <c r="F62" s="29" t="s">
         <v>24</v>
       </c>
@@ -4316,19 +4342,21 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63" s="26">
         <v>49</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C63" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D63" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E63" s="28"/>
+      <c r="E63" s="28" t="s">
+        <v>6</v>
+      </c>
       <c r="F63" s="29" t="s">
         <v>24</v>
       </c>
@@ -4337,14 +4365,14 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="26">
+      <c r="A64" s="1">
         <v>50</v>
       </c>
       <c r="B64" s="27" t="s">
-        <v>168</v>
+        <v>8</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>169</v>
+        <v>34</v>
       </c>
       <c r="D64" s="28" t="s">
         <v>49</v>
@@ -4362,10 +4390,10 @@
         <v>51</v>
       </c>
       <c r="B65" s="27" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="C65" s="28" t="s">
-        <v>36</v>
+        <v>169</v>
       </c>
       <c r="D65" s="28" t="s">
         <v>49</v>
@@ -4383,10 +4411,10 @@
         <v>52</v>
       </c>
       <c r="B66" s="27" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C66" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D66" s="28" t="s">
         <v>49</v>
@@ -4404,10 +4432,10 @@
         <v>53</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>283</v>
+        <v>3</v>
       </c>
       <c r="C67" s="28" t="s">
-        <v>285</v>
+        <v>35</v>
       </c>
       <c r="D67" s="28" t="s">
         <v>49</v>
@@ -4425,10 +4453,10 @@
         <v>54</v>
       </c>
       <c r="B68" s="27" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C68" s="28" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D68" s="28" t="s">
         <v>49</v>
@@ -4442,14 +4470,14 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="26">
+      <c r="A69" s="1">
         <v>55</v>
       </c>
       <c r="B69" s="27" t="s">
-        <v>9</v>
+        <v>284</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>37</v>
+        <v>286</v>
       </c>
       <c r="D69" s="28" t="s">
         <v>49</v>
@@ -4467,10 +4495,10 @@
         <v>56</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>4</v>
+        <v>287</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>38</v>
+        <v>292</v>
       </c>
       <c r="D70" s="28" t="s">
         <v>49</v>
@@ -4484,14 +4512,14 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71" s="26">
         <v>57</v>
       </c>
       <c r="B71" s="27" t="s">
-        <v>7</v>
+        <v>288</v>
       </c>
       <c r="C71" s="28" t="s">
-        <v>41</v>
+        <v>293</v>
       </c>
       <c r="D71" s="28" t="s">
         <v>49</v>
@@ -4505,14 +4533,14 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="26">
+      <c r="A72" s="1">
         <v>58</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>10</v>
+        <v>289</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>40</v>
+        <v>294</v>
       </c>
       <c r="D72" s="28" t="s">
         <v>49</v>
@@ -4530,10 +4558,10 @@
         <v>59</v>
       </c>
       <c r="B73" s="27" t="s">
-        <v>12</v>
+        <v>290</v>
       </c>
       <c r="C73" s="28" t="s">
-        <v>39</v>
+        <v>295</v>
       </c>
       <c r="D73" s="28" t="s">
         <v>49</v>
@@ -4547,42 +4575,42 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="26">
+      <c r="A74" s="1">
         <v>60</v>
       </c>
       <c r="B74" s="27" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="C74" s="28" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="D74" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E74" s="28"/>
       <c r="F74" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G74" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="26">
         <v>61</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="D75" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E75" s="28"/>
       <c r="F75" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G75" s="30" t="s">
         <v>62</v>
@@ -4593,38 +4621,38 @@
         <v>62</v>
       </c>
       <c r="B76" s="27" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C76" s="28" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="D76" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E76" s="28"/>
       <c r="F76" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G76" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="26">
+      <c r="A77" s="1">
         <v>63</v>
       </c>
       <c r="B77" s="27" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="C77" s="28" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
       <c r="D77" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E77" s="28"/>
       <c r="F77" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G77" s="30" t="s">
         <v>62</v>
@@ -4635,17 +4663,17 @@
         <v>64</v>
       </c>
       <c r="B78" s="27" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="C78" s="28" t="s">
-        <v>109</v>
+        <v>39</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E78" s="28"/>
       <c r="F78" s="29" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="G78" s="30" t="s">
         <v>62</v>
@@ -4656,10 +4684,10 @@
         <v>65</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="C79" s="28" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="D79" s="28" t="s">
         <v>49</v>
@@ -4677,10 +4705,10 @@
         <v>66</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="C80" s="28" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D80" s="28" t="s">
         <v>49</v>
@@ -4698,72 +4726,80 @@
         <v>67</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="C81" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D81" s="28"/>
+        <v>95</v>
+      </c>
+      <c r="D81" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E81" s="28"/>
       <c r="F81" s="29" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="G81" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="26">
+      <c r="A82" s="1">
         <v>68</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="C82" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D82" s="28"/>
+        <v>111</v>
+      </c>
+      <c r="D82" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E82" s="28"/>
       <c r="F82" s="29" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="G82" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="26">
         <v>69</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D83" s="28"/>
+        <v>109</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E83" s="28"/>
       <c r="F83" s="29" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="G83" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="26">
+      <c r="A84" s="1">
         <v>70</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D84" s="28"/>
+        <v>107</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E84" s="28"/>
       <c r="F84" s="29" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="G84" s="30" t="s">
         <v>62</v>
@@ -4774,15 +4810,17 @@
         <v>71</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>280</v>
-      </c>
-      <c r="D85" s="28"/>
+        <v>105</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E85" s="28"/>
       <c r="F85" s="29" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="G85" s="30" t="s">
         <v>62</v>
@@ -4793,10 +4831,10 @@
         <v>72</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>171</v>
+        <v>14</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>281</v>
+        <v>45</v>
       </c>
       <c r="D86" s="28"/>
       <c r="E86" s="28"/>
@@ -4812,10 +4850,10 @@
         <v>73</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>277</v>
+        <v>15</v>
       </c>
       <c r="C87" s="28" t="s">
-        <v>279</v>
+        <v>46</v>
       </c>
       <c r="D87" s="28"/>
       <c r="E87" s="28"/>
@@ -4831,10 +4869,10 @@
         <v>74</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>278</v>
+        <v>13</v>
       </c>
       <c r="C88" s="28" t="s">
-        <v>282</v>
+        <v>44</v>
       </c>
       <c r="D88" s="28"/>
       <c r="E88" s="28"/>
@@ -4846,18 +4884,16 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="26">
+      <c r="A89" s="1">
         <v>75</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D89" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D89" s="28"/>
       <c r="E89" s="28"/>
       <c r="F89" s="29" t="s">
         <v>25</v>
@@ -4871,14 +4907,12 @@
         <v>76</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="C90" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D90" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="D90" s="28"/>
       <c r="E90" s="28"/>
       <c r="F90" s="29" t="s">
         <v>25</v>
@@ -4888,18 +4922,16 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91" s="26">
         <v>77</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>43</v>
+        <v>171</v>
       </c>
       <c r="C91" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="D91" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="D91" s="28"/>
       <c r="E91" s="28"/>
       <c r="F91" s="29" t="s">
         <v>25</v>
@@ -4909,18 +4941,16 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="26">
+      <c r="A92" s="1">
         <v>78</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>18</v>
+        <v>277</v>
       </c>
       <c r="C92" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D92" s="28" t="s">
-        <v>50</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="D92" s="28"/>
       <c r="E92" s="28"/>
       <c r="F92" s="29" t="s">
         <v>25</v>
@@ -4934,14 +4964,12 @@
         <v>79</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>20</v>
+        <v>278</v>
       </c>
       <c r="C93" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D93" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>282</v>
+      </c>
+      <c r="D93" s="28"/>
       <c r="E93" s="28"/>
       <c r="F93" s="29" t="s">
         <v>25</v>
@@ -4951,42 +4979,42 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="26">
+      <c r="A94" s="1">
         <v>80</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>268</v>
+        <v>17</v>
       </c>
       <c r="C94" s="28" t="s">
-        <v>270</v>
+        <v>30</v>
       </c>
       <c r="D94" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E94" s="28"/>
       <c r="F94" s="29" t="s">
-        <v>272</v>
+        <v>25</v>
       </c>
       <c r="G94" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95" s="26">
         <v>81</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>269</v>
+        <v>19</v>
       </c>
       <c r="C95" s="28" t="s">
-        <v>271</v>
+        <v>27</v>
       </c>
       <c r="D95" s="28" t="s">
         <v>49</v>
       </c>
       <c r="E95" s="28"/>
       <c r="F95" s="29" t="s">
-        <v>272</v>
+        <v>25</v>
       </c>
       <c r="G95" s="30" t="s">
         <v>62</v>
@@ -4997,34 +5025,38 @@
         <v>82</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>273</v>
+        <v>43</v>
       </c>
       <c r="C96" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="D96" s="28"/>
+        <v>29</v>
+      </c>
+      <c r="D96" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E96" s="28"/>
       <c r="F96" s="29" t="s">
-        <v>272</v>
+        <v>25</v>
       </c>
       <c r="G96" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="26">
+      <c r="A97" s="1">
         <v>83</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>220</v>
+        <v>18</v>
       </c>
       <c r="C97" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="D97" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="D97" s="28" t="s">
+        <v>50</v>
+      </c>
       <c r="E97" s="28"/>
       <c r="F97" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G97" s="30" t="s">
         <v>62</v>
@@ -5035,15 +5067,17 @@
         <v>84</v>
       </c>
       <c r="B98" s="27" t="s">
-        <v>218</v>
+        <v>20</v>
       </c>
       <c r="C98" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D98" s="28"/>
+        <v>28</v>
+      </c>
+      <c r="D98" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E98" s="28"/>
       <c r="F98" s="29" t="s">
-        <v>236</v>
+        <v>25</v>
       </c>
       <c r="G98" s="30" t="s">
         <v>62</v>
@@ -5054,15 +5088,17 @@
         <v>85</v>
       </c>
       <c r="B99" s="27" t="s">
-        <v>249</v>
+        <v>268</v>
       </c>
       <c r="C99" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="D99" s="28"/>
+        <v>270</v>
+      </c>
+      <c r="D99" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E99" s="28"/>
       <c r="F99" s="29" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="G99" s="30" t="s">
         <v>62</v>
@@ -5073,15 +5109,17 @@
         <v>86</v>
       </c>
       <c r="B100" s="27" t="s">
-        <v>237</v>
+        <v>269</v>
       </c>
       <c r="C100" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="D100" s="28"/>
+        <v>271</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E100" s="28"/>
       <c r="F100" s="29" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="G100" s="30" t="s">
         <v>62</v>
@@ -5092,29 +5130,29 @@
         <v>87</v>
       </c>
       <c r="B101" s="27" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
       <c r="C101" s="28" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="D101" s="28"/>
       <c r="E101" s="28"/>
       <c r="F101" s="29" t="s">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="G101" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="26">
+      <c r="A102" s="1">
         <v>88</v>
       </c>
       <c r="B102" s="27" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C102" s="28" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="D102" s="28"/>
       <c r="E102" s="28"/>
@@ -5126,14 +5164,14 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+      <c r="A103" s="26">
         <v>89</v>
       </c>
       <c r="B103" s="27" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="C103" s="28" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D103" s="28"/>
       <c r="E103" s="28"/>
@@ -5145,18 +5183,16 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="26">
+      <c r="A104" s="1">
         <v>90</v>
       </c>
       <c r="B104" s="27" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="C104" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="D104" s="28" t="s">
-        <v>50</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="D104" s="28"/>
       <c r="E104" s="28"/>
       <c r="F104" s="29" t="s">
         <v>236</v>
@@ -5170,10 +5206,10 @@
         <v>91</v>
       </c>
       <c r="B105" s="27" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C105" s="28" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -5189,10 +5225,10 @@
         <v>92</v>
       </c>
       <c r="B106" s="27" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="C106" s="28" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -5208,10 +5244,10 @@
         <v>93</v>
       </c>
       <c r="B107" s="27" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="C107" s="28" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="D107" s="28"/>
       <c r="E107" s="28"/>
@@ -5227,10 +5263,10 @@
         <v>94</v>
       </c>
       <c r="B108" s="27" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="C108" s="28" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="D108" s="28"/>
       <c r="E108" s="28"/>
@@ -5242,16 +5278,18 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="26">
+      <c r="A109" s="1">
         <v>95</v>
       </c>
       <c r="B109" s="27" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="C109" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="D109" s="28"/>
+        <v>233</v>
+      </c>
+      <c r="D109" s="28" t="s">
+        <v>50</v>
+      </c>
       <c r="E109" s="28"/>
       <c r="F109" s="29" t="s">
         <v>236</v>
@@ -5265,10 +5303,10 @@
         <v>96</v>
       </c>
       <c r="B110" s="27" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C110" s="28" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -5280,14 +5318,14 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="A111" s="26">
         <v>97</v>
       </c>
       <c r="B111" s="27" t="s">
-        <v>275</v>
+        <v>212</v>
       </c>
       <c r="C111" s="28" t="s">
-        <v>276</v>
+        <v>213</v>
       </c>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -5299,14 +5337,14 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="26">
+      <c r="A112" s="1">
         <v>98</v>
       </c>
       <c r="B112" s="27" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="C112" s="28" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -5322,10 +5360,10 @@
         <v>99</v>
       </c>
       <c r="B113" s="27" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="C113" s="28" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -5337,18 +5375,16 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="26">
+      <c r="A114" s="1">
         <v>100</v>
       </c>
       <c r="B114" s="27" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C114" s="28" t="s">
-        <v>251</v>
-      </c>
-      <c r="D114" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="D114" s="28"/>
       <c r="E114" s="28"/>
       <c r="F114" s="29" t="s">
         <v>236</v>
@@ -5358,14 +5394,14 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1">
+      <c r="A115" s="26">
         <v>101</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C115" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D115" s="28"/>
       <c r="E115" s="28"/>
@@ -5381,10 +5417,10 @@
         <v>102</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="C116" s="28" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="D116" s="28"/>
       <c r="E116" s="28"/>
@@ -5396,14 +5432,14 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="26">
+      <c r="A117" s="1">
         <v>103</v>
       </c>
       <c r="B117" s="27" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C117" s="28" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D117" s="28"/>
       <c r="E117" s="28"/>
@@ -5419,10 +5455,10 @@
         <v>104</v>
       </c>
       <c r="B118" s="27" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="C118" s="28" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="D118" s="28"/>
       <c r="E118" s="28"/>
@@ -5438,12 +5474,14 @@
         <v>105</v>
       </c>
       <c r="B119" s="27" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
       <c r="C119" s="28" t="s">
-        <v>267</v>
-      </c>
-      <c r="D119" s="28"/>
+        <v>251</v>
+      </c>
+      <c r="D119" s="28" t="s">
+        <v>49</v>
+      </c>
       <c r="E119" s="28"/>
       <c r="F119" s="29" t="s">
         <v>236</v>
@@ -5457,10 +5495,10 @@
         <v>106</v>
       </c>
       <c r="B120" s="27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C120" s="28" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D120" s="28"/>
       <c r="E120" s="28"/>
@@ -5476,76 +5514,171 @@
         <v>107</v>
       </c>
       <c r="B121" s="27" t="s">
-        <v>206</v>
+        <v>261</v>
       </c>
       <c r="C121" s="28" t="s">
-        <v>207</v>
+        <v>264</v>
       </c>
       <c r="D121" s="28"/>
       <c r="E121" s="28"/>
       <c r="F121" s="29" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G121" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="26">
+      <c r="A122" s="1">
         <v>108</v>
       </c>
       <c r="B122" s="27" t="s">
-        <v>210</v>
+        <v>262</v>
       </c>
       <c r="C122" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="D122" s="28" t="s">
-        <v>49</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="D122" s="28"/>
       <c r="E122" s="28"/>
       <c r="F122" s="29" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G122" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
+      <c r="A123" s="26">
         <v>109</v>
       </c>
       <c r="B123" s="27" t="s">
-        <v>208</v>
+        <v>247</v>
       </c>
       <c r="C123" s="28" t="s">
-        <v>209</v>
+        <v>253</v>
       </c>
       <c r="D123" s="28"/>
       <c r="E123" s="28"/>
       <c r="F123" s="29" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="G123" s="30" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="26">
+      <c r="A124" s="1">
         <v>110</v>
       </c>
       <c r="B124" s="27" t="s">
-        <v>204</v>
+        <v>266</v>
       </c>
       <c r="C124" s="28" t="s">
-        <v>205</v>
+        <v>267</v>
       </c>
       <c r="D124" s="28"/>
       <c r="E124" s="28"/>
       <c r="F124" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="G124" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>111</v>
+      </c>
+      <c r="B125" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="C125" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="D125" s="28"/>
+      <c r="E125" s="28"/>
+      <c r="F125" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="G125" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>112</v>
+      </c>
+      <c r="B126" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="C126" s="28" t="s">
+        <v>207</v>
+      </c>
+      <c r="D126" s="28"/>
+      <c r="E126" s="28"/>
+      <c r="F126" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="G124" s="30" t="s">
+      <c r="G126" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="26">
+        <v>113</v>
+      </c>
+      <c r="B127" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="C127" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D127" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E127" s="28"/>
+      <c r="F127" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="G127" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>114</v>
+      </c>
+      <c r="B128" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C128" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D128" s="28"/>
+      <c r="E128" s="28"/>
+      <c r="F128" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="G128" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>115</v>
+      </c>
+      <c r="B129" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C129" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D129" s="28"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="29" t="s">
+        <v>235</v>
+      </c>
+      <c r="G129" s="30" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>